<commit_message>
notebook for conversion to id
</commit_message>
<xml_diff>
--- a/files/CH_ISCO_19.xlsx
+++ b/files/CH_ISCO_19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janjorg/Documents/bachelorarbeit_code/bachelorarbeit/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA15D89-4006-D040-B726-9840267D511C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{410380DD-9F9E-D84C-90B8-DF4156E8B0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34060" windowHeight="26560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34060" yWindow="500" windowWidth="34060" windowHeight="26560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CH_ISCO_19" sheetId="1" r:id="rId1"/>
@@ -7458,9 +7458,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G1490"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>